<commit_message>
Ven 17 aoû 2018 09:04:59 GMT _
</commit_message>
<xml_diff>
--- a/web/presences.xlsx
+++ b/web/presences.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Heure</t>
   </si>
@@ -29,22 +29,61 @@
     <t>Type</t>
   </si>
   <si>
-    <t>17:49</t>
+    <t>17:55</t>
+  </si>
+  <si>
+    <t>Epiphanie Adoboè</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Départ</t>
+  </si>
+  <si>
+    <t>17:40</t>
+  </si>
+  <si>
+    <t>Akouété Kangnivi</t>
+  </si>
+  <si>
+    <t>Juriste</t>
+  </si>
+  <si>
+    <t>17:35</t>
+  </si>
+  <si>
+    <t>Ibrahim Kodjo</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>16:51</t>
+  </si>
+  <si>
+    <t>Amah Kwatcha</t>
+  </si>
+  <si>
+    <t>16:45</t>
   </si>
   <si>
     <t>Abi Conrad</t>
   </si>
   <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>Départ</t>
-  </si>
-  <si>
-    <t>Amah Kwatcha</t>
-  </si>
-  <si>
-    <t>17:35</t>
+    <t>Abalo Afi</t>
+  </si>
+  <si>
+    <t>16:38</t>
+  </si>
+  <si>
+    <t>Romuald Gagnon</t>
+  </si>
+  <si>
+    <t>PHOTOGRAPHE</t>
+  </si>
+  <si>
+    <t>16:15</t>
   </si>
   <si>
     <t>Adjovi Abla</t>
@@ -53,28 +92,16 @@
     <t>Developpeur</t>
   </si>
   <si>
-    <t>17:25</t>
-  </si>
-  <si>
-    <t>Romuald Gagnon</t>
-  </si>
-  <si>
-    <t>PHOTOGRAPHE</t>
-  </si>
-  <si>
-    <t>17:10</t>
-  </si>
-  <si>
-    <t>Epiphanie Adoboè</t>
-  </si>
-  <si>
-    <t>16:38</t>
-  </si>
-  <si>
-    <t>Akouété Kangnivi</t>
-  </si>
-  <si>
-    <t>Juriste</t>
+    <t>13:51</t>
+  </si>
+  <si>
+    <t>Fin pause</t>
+  </si>
+  <si>
+    <t>13:45</t>
+  </si>
+  <si>
+    <t>13:22</t>
   </si>
   <si>
     <t>Napo Kuvor</t>
@@ -83,52 +110,34 @@
     <t>Mecanicien</t>
   </si>
   <si>
-    <t>16:22</t>
-  </si>
-  <si>
-    <t>Ibrahim Kodjo</t>
-  </si>
-  <si>
-    <t>Web</t>
-  </si>
-  <si>
-    <t>16:07</t>
-  </si>
-  <si>
-    <t>Abalo Afi</t>
-  </si>
-  <si>
-    <t>14:49</t>
-  </si>
-  <si>
-    <t>Fin pause</t>
-  </si>
-  <si>
-    <t>13:38</t>
-  </si>
-  <si>
-    <t>12:49</t>
+    <t>11:51</t>
   </si>
   <si>
     <t>Pause</t>
   </si>
   <si>
-    <t>11:38</t>
-  </si>
-  <si>
-    <t>08:49</t>
+    <t>11:45</t>
+  </si>
+  <si>
+    <t>11:22</t>
+  </si>
+  <si>
+    <t>08:55</t>
   </si>
   <si>
     <t>Arrivée</t>
   </si>
   <si>
+    <t>08:40</t>
+  </si>
+  <si>
     <t>08:35</t>
   </si>
   <si>
-    <t>08:25</t>
-  </si>
-  <si>
-    <t>08:10</t>
+    <t>07:51</t>
+  </si>
+  <si>
+    <t>07:45</t>
   </si>
   <si>
     <t>07:38</t>
@@ -137,7 +146,7 @@
     <t>07:22</t>
   </si>
   <si>
-    <t>07:07</t>
+    <t>07:15</t>
   </si>
 </sst>
 </file>
@@ -476,7 +485,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,13 +523,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -528,13 +537,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -542,13 +551,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -556,10 +565,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -570,13 +579,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -584,7 +593,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -615,13 +624,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -629,186 +638,186 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
         <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
@@ -817,21 +826,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ven 17 aoû 2018 11:47:38 GMT _
</commit_message>
<xml_diff>
--- a/web/presences.xlsx
+++ b/web/presences.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Heure</t>
   </si>
@@ -32,16 +32,64 @@
     <t>17:55</t>
   </si>
   <si>
+    <t>Adjovi Abla</t>
+  </si>
+  <si>
+    <t>Developpeur</t>
+  </si>
+  <si>
+    <t>Départ</t>
+  </si>
+  <si>
+    <t>17:54</t>
+  </si>
+  <si>
+    <t>Napo Kuvor</t>
+  </si>
+  <si>
+    <t>Mecanicien</t>
+  </si>
+  <si>
+    <t>17:48</t>
+  </si>
+  <si>
+    <t>Ibrahim Kodjo</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>17:43</t>
+  </si>
+  <si>
+    <t>Amah Kwatcha</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>16:48</t>
+  </si>
+  <si>
+    <t>Romuald Gagnon</t>
+  </si>
+  <si>
+    <t>PHOTOGRAPHE</t>
+  </si>
+  <si>
+    <t>16:39</t>
+  </si>
+  <si>
+    <t>Abalo Afi</t>
+  </si>
+  <si>
+    <t>16:23</t>
+  </si>
+  <si>
     <t>Epiphanie Adoboè</t>
   </si>
   <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>Départ</t>
-  </si>
-  <si>
-    <t>17:40</t>
+    <t>16:19</t>
   </si>
   <si>
     <t>Akouété Kangnivi</t>
@@ -50,76 +98,31 @@
     <t>Juriste</t>
   </si>
   <si>
-    <t>17:35</t>
-  </si>
-  <si>
-    <t>Ibrahim Kodjo</t>
-  </si>
-  <si>
-    <t>Web</t>
-  </si>
-  <si>
-    <t>16:51</t>
-  </si>
-  <si>
-    <t>Amah Kwatcha</t>
-  </si>
-  <si>
-    <t>16:45</t>
+    <t>14:54</t>
+  </si>
+  <si>
+    <t>Fin pause</t>
+  </si>
+  <si>
+    <t>14:43</t>
+  </si>
+  <si>
+    <t>13:07</t>
   </si>
   <si>
     <t>Abi Conrad</t>
   </si>
   <si>
-    <t>Abalo Afi</t>
-  </si>
-  <si>
-    <t>16:38</t>
-  </si>
-  <si>
-    <t>Romuald Gagnon</t>
-  </si>
-  <si>
-    <t>PHOTOGRAPHE</t>
-  </si>
-  <si>
-    <t>16:15</t>
-  </si>
-  <si>
-    <t>Adjovi Abla</t>
-  </si>
-  <si>
-    <t>Developpeur</t>
-  </si>
-  <si>
-    <t>13:51</t>
-  </si>
-  <si>
-    <t>Fin pause</t>
-  </si>
-  <si>
-    <t>13:45</t>
-  </si>
-  <si>
-    <t>13:22</t>
-  </si>
-  <si>
-    <t>Napo Kuvor</t>
-  </si>
-  <si>
-    <t>Mecanicien</t>
-  </si>
-  <si>
-    <t>11:51</t>
+    <t>12:54</t>
   </si>
   <si>
     <t>Pause</t>
   </si>
   <si>
-    <t>11:45</t>
-  </si>
-  <si>
-    <t>11:22</t>
+    <t>12:43</t>
+  </si>
+  <si>
+    <t>11:07</t>
   </si>
   <si>
     <t>08:55</t>
@@ -128,25 +131,28 @@
     <t>Arrivée</t>
   </si>
   <si>
-    <t>08:40</t>
-  </si>
-  <si>
-    <t>08:35</t>
-  </si>
-  <si>
-    <t>07:51</t>
-  </si>
-  <si>
-    <t>07:45</t>
-  </si>
-  <si>
-    <t>07:38</t>
-  </si>
-  <si>
-    <t>07:22</t>
-  </si>
-  <si>
-    <t>07:15</t>
+    <t>08:54</t>
+  </si>
+  <si>
+    <t>08:48</t>
+  </si>
+  <si>
+    <t>08:43</t>
+  </si>
+  <si>
+    <t>07:48</t>
+  </si>
+  <si>
+    <t>07:39</t>
+  </si>
+  <si>
+    <t>07:23</t>
+  </si>
+  <si>
+    <t>07:19</t>
+  </si>
+  <si>
+    <t>07:07</t>
   </si>
 </sst>
 </file>
@@ -557,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -565,13 +571,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -579,13 +585,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -593,13 +599,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -607,13 +613,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -621,91 +627,91 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -714,12 +720,12 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -728,12 +734,12 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -742,91 +748,91 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>